<commit_message>
Variable PWM intensity Masive for 1s
</commit_message>
<xml_diff>
--- a/Times and %.xlsx
+++ b/Times and %.xlsx
@@ -61,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,16 +87,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -408,379 +418,388 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="A12:K12"/>
+      <selection activeCell="L13" sqref="A1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1">
         <v>255</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>ROUND(C3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>ROUND(D3,0)</f>
         <v>255</v>
       </c>
-      <c r="C3">
-        <f>D1*D3</f>
+      <c r="D3">
+        <f>E1*E3</f>
         <v>255</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
-        <f>19+(19*(1-D3))</f>
-        <v>19</v>
-      </c>
-      <c r="F3" s="1">
-        <f>ROUND(E3,0)</f>
-        <v>19</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3">
+      <c r="I3" s="1"/>
+      <c r="J3">
         <v>19</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>255</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>997</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A13" si="0">ROUND(C4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B12" si="0">ROUND(D4,0)</f>
         <v>230</v>
       </c>
-      <c r="C4">
-        <f>255*D4</f>
+      <c r="D4">
+        <f>255*E4</f>
         <v>229.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.9</v>
       </c>
-      <c r="E4" s="1">
-        <f>19+(19*(1-D4))</f>
-        <v>20.9</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ref="F4:F13" si="1">ROUND(E4,0)</f>
-        <v>21</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="C5">
-        <f>255*D5</f>
+      <c r="D5">
+        <f>255*E5</f>
         <v>204</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.8</v>
       </c>
-      <c r="E5" s="1">
-        <f>19+(19*(1-D5))</f>
-        <v>22.799999999999997</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>179</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C13" si="2">255*D6</f>
+        <v>180</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D12" si="1">255*E6</f>
         <v>178.5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.7</v>
       </c>
-      <c r="E6" s="1">
-        <f>19+(19*(1-D6))</f>
-        <v>24.700000000000003</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>153</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
         <v>153</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0.6</v>
       </c>
-      <c r="E7" s="1">
-        <f>19+(19*(1-D7))</f>
-        <v>26.6</v>
-      </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="I7" s="1">
+        <v>32</v>
+      </c>
+      <c r="L7">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="2">
         <v>129</v>
       </c>
-      <c r="C8" s="3">
-        <f t="shared" si="2"/>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
         <v>127.5</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="3">
         <v>0.5</v>
       </c>
-      <c r="E8" s="4">
-        <f>19+(19*(D8))</f>
-        <v>28.5</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3">
         <v>39</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="3">
         <v>39</v>
       </c>
-      <c r="I8" s="3">
-        <f>I3*2</f>
+      <c r="J8" s="2">
+        <f>J3*2</f>
         <v>38</v>
       </c>
-      <c r="J8" s="3">
-        <f>J3/2</f>
+      <c r="K8" s="2">
+        <f>K3/2</f>
         <v>127.5</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="2">
         <v>997.1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="2"/>
+      <c r="C9" s="2">
         <v>102</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="E9" s="3">
         <v>0.4</v>
       </c>
-      <c r="E9" s="1">
-        <f>19+(19*(1-D9))</f>
-        <v>30.4</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
+        <v>50</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="2"/>
+      <c r="C10" s="2">
+        <v>77</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
         <v>76.5</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="3">
         <v>0.3</v>
       </c>
-      <c r="E10" s="1">
-        <f>19+(19*(1/D10))</f>
-        <v>82.333333333333343</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3">
+        <v>66</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
+        <f>19*5</f>
+        <v>95</v>
+      </c>
+      <c r="I11" s="3">
+        <v>99</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
         <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3">
+        <v>195</v>
+      </c>
+      <c r="I12" s="3">
+        <v>195</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <f>ROUND(D13,0)</f>
         <v>64</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="2"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5">
+        <f>255*E13</f>
         <v>63.75</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E13" s="6">
         <v>0.25</v>
       </c>
-      <c r="E11" s="1">
-        <f>19+(19*(1-D11))</f>
+      <c r="F13" s="6">
+        <f>19+(19*(1-E13))</f>
         <v>33.25</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
+      <c r="G13" s="6">
+        <f>ROUND(F13,0)</f>
         <v>33</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H13" s="6">
         <f>19*4</f>
         <v>76</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11">
+      <c r="I13" s="6"/>
+      <c r="J13" s="5">
         <f>19*4</f>
         <v>76</v>
       </c>
-      <c r="J11">
+      <c r="K13" s="5">
         <f>255/6</f>
         <v>42.5</v>
       </c>
-      <c r="K11">
+      <c r="L13" s="5">
         <v>933</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="4">
-        <f>19+(19*(1-D12))</f>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="G12" s="4">
-        <f>19*5</f>
-        <v>95</v>
-      </c>
-      <c r="H12" s="4">
-        <v>99</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3">
-        <v>1.006</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
-        <f t="shared" si="2"/>
-        <v>25.5</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="4">
-        <f>19+(19*(1-D13))</f>
-        <v>36.1</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="G13" s="4">
-        <v>195</v>
-      </c>
-      <c r="H13" s="4">
-        <v>195</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3">
-        <v>1.002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>